<commit_message>
update rpa shelf price template
</commit_message>
<xml_diff>
--- a/Module.Frontend.TPM/Content/Templates/ActualShelfPriceTemplate.xlsx
+++ b/Module.Frontend.TPM/Content/Templates/ActualShelfPriceTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25219"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30.10.2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\М\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB8A339-D35B-4FBF-ABBE-8EF5E306F0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="4245" yWindow="4245" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -63,15 +64,15 @@
     <t>Document number</t>
   </si>
   <si>
+    <t>VP</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
     <t>TPR</t>
   </si>
   <si>
-    <t>VP</t>
-  </si>
-  <si>
     <t>2+1</t>
   </si>
   <si>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,11 +411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +454,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{ED53B5C9-AC7B-41C4-BE27-FEBFC6723A69}">
       <formula1>INDIRECT(B2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -462,7 +463,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0B8A2378-A95E-4D85-A1D1-CDE0CA6DE905}">
           <x14:formula1>
             <xm:f>Mechanics!$A:$A</xm:f>
           </x14:formula1>
@@ -475,7 +476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC80930-7F4F-4A05-A0B9-C5579139E38B}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
@@ -484,17 +485,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829C839B-7FA0-4316-B275-2071017C7F76}">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
@@ -556,15 +557,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Краткое_x0020_описание xmlns="583145ed-b998-4802-bdfd-b0ec64ffe47d" xsi:nil="true"/>
@@ -579,7 +571,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008BD6AFE2CAF68846A90AF41F02AA6078" ma:contentTypeVersion="50" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d98a57736acbe81ebd48d911a51b45cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="583145ed-b998-4802-bdfd-b0ec64ffe47d" xmlns:ns3="e45562e1-71fb-4bba-8dff-84d3788fc1cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57b2f41c826d6401cab8db36b557d145" ns2:_="" ns3:_="">
     <xsd:import namespace="583145ed-b998-4802-bdfd-b0ec64ffe47d"/>
@@ -818,32 +810,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{620060DD-3157-4681-92C6-CB266EBFA7BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F26BB653-72E2-4E52-B82A-F16278DF79C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="583145ed-b998-4802-bdfd-b0ec64ffe47d"/>
+    <ds:schemaRef ds:uri="e45562e1-71fb-4bba-8dff-84d3788fc1cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F26BB653-72E2-4E52-B82A-F16278DF79C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="583145ed-b998-4802-bdfd-b0ec64ffe47d"/>
-    <ds:schemaRef ds:uri="e45562e1-71fb-4bba-8dff-84d3788fc1cf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B711D58C-4AE3-4068-9C44-7A803B5E09D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -860,4 +847,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{620060DD-3157-4681-92C6-CB266EBFA7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>